<commit_message>
New plots with error bars
</commit_message>
<xml_diff>
--- a/Interleaved-Christian/evap_N_circ_cross_couter_flow/Tuning/superheat/effectivness.xlsx
+++ b/Interleaved-Christian/evap_N_circ_cross_couter_flow/Tuning/superheat/effectivness.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammarbahman/Desktop/Eclipse workspace/Trunk/Interleaved-Christian/evap_N_circ_cross_couter_flow/Tuning/superheat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Purdue\PhD\Journals\Interleaved paper\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="16780" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14355" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>effectivness</t>
   </si>
@@ -367,17 +362,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,7 +386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -405,7 +400,7 @@
         <v>0.54149999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -419,7 +414,7 @@
         <v>0.44550000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -433,7 +428,7 @@
         <v>0.52270000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -447,7 +442,7 @@
         <v>0.48759999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -461,7 +456,7 @@
         <v>0.41089999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -475,7 +470,7 @@
         <v>0.39140000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -489,7 +484,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -501,6 +496,147 @@
       </c>
       <c r="D9">
         <v>0.31040000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.52859999999999996</v>
+      </c>
+      <c r="C2">
+        <v>0.51</v>
+      </c>
+      <c r="D2">
+        <v>0.57110000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.43630000000000002</v>
+      </c>
+      <c r="C3">
+        <v>0.42820000000000003</v>
+      </c>
+      <c r="D3">
+        <v>0.45250000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.49769999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.50690000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.57050000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="C5">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.56069999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.3972</v>
+      </c>
+      <c r="C6">
+        <v>0.40260000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.43240000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.40039999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.39860000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.44550000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0.37930000000000003</v>
+      </c>
+      <c r="C8">
+        <v>0.37240000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.3004</v>
+      </c>
+      <c r="C9">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.32150000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>